<commit_message>
update data fetching example
</commit_message>
<xml_diff>
--- a/data/treasury/daily_treasury_long_term_rate.xlsx
+++ b/data/treasury/daily_treasury_long_term_rate.xlsx
@@ -25,754 +25,754 @@
     <t>TREASURY 20-Yr CMT</t>
   </si>
   <si>
-    <t>2016-12-30</t>
-  </si>
-  <si>
-    <t>2016-12-29</t>
-  </si>
-  <si>
-    <t>2016-12-28</t>
-  </si>
-  <si>
-    <t>2016-12-27</t>
-  </si>
-  <si>
-    <t>2016-12-23</t>
-  </si>
-  <si>
-    <t>2016-12-22</t>
-  </si>
-  <si>
-    <t>2016-12-21</t>
-  </si>
-  <si>
-    <t>2016-12-20</t>
-  </si>
-  <si>
-    <t>2016-12-19</t>
-  </si>
-  <si>
-    <t>2016-12-16</t>
-  </si>
-  <si>
-    <t>2016-12-15</t>
-  </si>
-  <si>
-    <t>2016-12-14</t>
-  </si>
-  <si>
-    <t>2016-12-13</t>
-  </si>
-  <si>
-    <t>2016-12-12</t>
-  </si>
-  <si>
-    <t>2016-12-09</t>
-  </si>
-  <si>
-    <t>2016-12-08</t>
-  </si>
-  <si>
-    <t>2016-12-07</t>
-  </si>
-  <si>
-    <t>2016-12-06</t>
-  </si>
-  <si>
-    <t>2016-12-05</t>
-  </si>
-  <si>
-    <t>2016-12-02</t>
-  </si>
-  <si>
-    <t>2016-12-01</t>
-  </si>
-  <si>
-    <t>2016-11-30</t>
-  </si>
-  <si>
-    <t>2016-11-29</t>
-  </si>
-  <si>
-    <t>2016-11-28</t>
-  </si>
-  <si>
-    <t>2016-11-25</t>
-  </si>
-  <si>
-    <t>2016-11-23</t>
-  </si>
-  <si>
-    <t>2016-11-22</t>
-  </si>
-  <si>
-    <t>2016-11-21</t>
-  </si>
-  <si>
-    <t>2016-11-18</t>
-  </si>
-  <si>
-    <t>2016-11-17</t>
-  </si>
-  <si>
-    <t>2016-11-16</t>
-  </si>
-  <si>
-    <t>2016-11-15</t>
-  </si>
-  <si>
-    <t>2016-11-14</t>
-  </si>
-  <si>
-    <t>2016-11-10</t>
-  </si>
-  <si>
-    <t>2016-11-09</t>
-  </si>
-  <si>
-    <t>2016-11-08</t>
-  </si>
-  <si>
-    <t>2016-11-07</t>
-  </si>
-  <si>
-    <t>2016-11-04</t>
-  </si>
-  <si>
-    <t>2016-11-03</t>
-  </si>
-  <si>
-    <t>2016-11-02</t>
-  </si>
-  <si>
-    <t>2016-11-01</t>
-  </si>
-  <si>
-    <t>2016-10-31</t>
-  </si>
-  <si>
-    <t>2016-10-28</t>
-  </si>
-  <si>
-    <t>2016-10-27</t>
-  </si>
-  <si>
-    <t>2016-10-26</t>
-  </si>
-  <si>
-    <t>2016-10-25</t>
-  </si>
-  <si>
-    <t>2016-10-24</t>
-  </si>
-  <si>
-    <t>2016-10-21</t>
-  </si>
-  <si>
-    <t>2016-10-20</t>
-  </si>
-  <si>
-    <t>2016-10-19</t>
-  </si>
-  <si>
-    <t>2016-10-18</t>
-  </si>
-  <si>
-    <t>2016-10-17</t>
-  </si>
-  <si>
-    <t>2016-10-14</t>
-  </si>
-  <si>
-    <t>2016-10-13</t>
-  </si>
-  <si>
-    <t>2016-10-12</t>
-  </si>
-  <si>
-    <t>2016-10-11</t>
-  </si>
-  <si>
-    <t>2016-10-07</t>
-  </si>
-  <si>
-    <t>2016-10-06</t>
-  </si>
-  <si>
-    <t>2016-10-05</t>
-  </si>
-  <si>
-    <t>2016-10-04</t>
-  </si>
-  <si>
-    <t>2016-10-03</t>
-  </si>
-  <si>
-    <t>2016-09-30</t>
-  </si>
-  <si>
-    <t>2016-09-29</t>
-  </si>
-  <si>
-    <t>2016-09-28</t>
-  </si>
-  <si>
-    <t>2016-09-27</t>
-  </si>
-  <si>
-    <t>2016-09-26</t>
-  </si>
-  <si>
-    <t>2016-09-23</t>
-  </si>
-  <si>
-    <t>2016-09-22</t>
-  </si>
-  <si>
-    <t>2016-09-21</t>
-  </si>
-  <si>
-    <t>2016-09-20</t>
-  </si>
-  <si>
-    <t>2016-09-19</t>
-  </si>
-  <si>
-    <t>2016-09-16</t>
-  </si>
-  <si>
-    <t>2016-09-15</t>
-  </si>
-  <si>
-    <t>2016-09-14</t>
-  </si>
-  <si>
-    <t>2016-09-13</t>
-  </si>
-  <si>
-    <t>2016-09-12</t>
-  </si>
-  <si>
-    <t>2016-09-09</t>
-  </si>
-  <si>
-    <t>2016-09-08</t>
-  </si>
-  <si>
-    <t>2016-09-07</t>
-  </si>
-  <si>
-    <t>2016-09-06</t>
-  </si>
-  <si>
-    <t>2016-09-02</t>
-  </si>
-  <si>
-    <t>2016-09-01</t>
-  </si>
-  <si>
-    <t>2016-08-31</t>
-  </si>
-  <si>
-    <t>2016-08-30</t>
-  </si>
-  <si>
-    <t>2016-08-29</t>
-  </si>
-  <si>
-    <t>2016-08-26</t>
-  </si>
-  <si>
-    <t>2016-08-25</t>
-  </si>
-  <si>
-    <t>2016-08-24</t>
-  </si>
-  <si>
-    <t>2016-08-23</t>
-  </si>
-  <si>
-    <t>2016-08-22</t>
-  </si>
-  <si>
-    <t>2016-08-19</t>
-  </si>
-  <si>
-    <t>2016-08-18</t>
-  </si>
-  <si>
-    <t>2016-08-17</t>
-  </si>
-  <si>
-    <t>2016-08-16</t>
-  </si>
-  <si>
-    <t>2016-08-15</t>
-  </si>
-  <si>
-    <t>2016-08-12</t>
-  </si>
-  <si>
-    <t>2016-08-11</t>
-  </si>
-  <si>
-    <t>2016-08-10</t>
-  </si>
-  <si>
-    <t>2016-08-09</t>
-  </si>
-  <si>
-    <t>2016-08-08</t>
-  </si>
-  <si>
-    <t>2016-08-05</t>
-  </si>
-  <si>
-    <t>2016-08-04</t>
-  </si>
-  <si>
-    <t>2016-08-03</t>
-  </si>
-  <si>
-    <t>2016-08-02</t>
-  </si>
-  <si>
-    <t>2016-08-01</t>
-  </si>
-  <si>
-    <t>2016-07-29</t>
-  </si>
-  <si>
-    <t>2016-07-28</t>
-  </si>
-  <si>
-    <t>2016-07-27</t>
-  </si>
-  <si>
-    <t>2016-07-26</t>
-  </si>
-  <si>
-    <t>2016-07-25</t>
-  </si>
-  <si>
-    <t>2016-07-22</t>
-  </si>
-  <si>
-    <t>2016-07-21</t>
-  </si>
-  <si>
-    <t>2016-07-20</t>
-  </si>
-  <si>
-    <t>2016-07-19</t>
-  </si>
-  <si>
-    <t>2016-07-18</t>
-  </si>
-  <si>
-    <t>2016-07-15</t>
-  </si>
-  <si>
-    <t>2016-07-14</t>
-  </si>
-  <si>
-    <t>2016-07-13</t>
-  </si>
-  <si>
-    <t>2016-07-12</t>
-  </si>
-  <si>
-    <t>2016-07-11</t>
-  </si>
-  <si>
-    <t>2016-07-08</t>
-  </si>
-  <si>
-    <t>2016-07-07</t>
-  </si>
-  <si>
-    <t>2016-07-06</t>
-  </si>
-  <si>
-    <t>2016-07-05</t>
-  </si>
-  <si>
-    <t>2016-07-01</t>
-  </si>
-  <si>
-    <t>2016-06-30</t>
-  </si>
-  <si>
-    <t>2016-06-29</t>
-  </si>
-  <si>
-    <t>2016-06-28</t>
-  </si>
-  <si>
-    <t>2016-06-27</t>
-  </si>
-  <si>
-    <t>2016-06-24</t>
-  </si>
-  <si>
-    <t>2016-06-23</t>
-  </si>
-  <si>
-    <t>2016-06-22</t>
-  </si>
-  <si>
-    <t>2016-06-21</t>
-  </si>
-  <si>
-    <t>2016-06-20</t>
-  </si>
-  <si>
-    <t>2016-06-17</t>
-  </si>
-  <si>
-    <t>2016-06-16</t>
-  </si>
-  <si>
-    <t>2016-06-15</t>
-  </si>
-  <si>
-    <t>2016-06-14</t>
-  </si>
-  <si>
-    <t>2016-06-13</t>
-  </si>
-  <si>
-    <t>2016-06-10</t>
-  </si>
-  <si>
-    <t>2016-06-09</t>
-  </si>
-  <si>
-    <t>2016-06-08</t>
-  </si>
-  <si>
-    <t>2016-06-07</t>
-  </si>
-  <si>
-    <t>2016-06-06</t>
-  </si>
-  <si>
-    <t>2016-06-03</t>
-  </si>
-  <si>
-    <t>2016-06-02</t>
-  </si>
-  <si>
-    <t>2016-06-01</t>
-  </si>
-  <si>
-    <t>2016-05-31</t>
-  </si>
-  <si>
-    <t>2016-05-27</t>
-  </si>
-  <si>
-    <t>2016-05-26</t>
-  </si>
-  <si>
-    <t>2016-05-25</t>
-  </si>
-  <si>
-    <t>2016-05-24</t>
-  </si>
-  <si>
-    <t>2016-05-23</t>
-  </si>
-  <si>
-    <t>2016-05-20</t>
-  </si>
-  <si>
-    <t>2016-05-19</t>
-  </si>
-  <si>
-    <t>2016-05-18</t>
-  </si>
-  <si>
-    <t>2016-05-17</t>
-  </si>
-  <si>
-    <t>2016-05-16</t>
-  </si>
-  <si>
-    <t>2016-05-13</t>
-  </si>
-  <si>
-    <t>2016-05-12</t>
-  </si>
-  <si>
-    <t>2016-05-11</t>
-  </si>
-  <si>
-    <t>2016-05-10</t>
-  </si>
-  <si>
-    <t>2016-05-09</t>
-  </si>
-  <si>
-    <t>2016-05-06</t>
-  </si>
-  <si>
-    <t>2016-05-05</t>
-  </si>
-  <si>
-    <t>2016-05-04</t>
-  </si>
-  <si>
-    <t>2016-05-03</t>
-  </si>
-  <si>
-    <t>2016-05-02</t>
-  </si>
-  <si>
-    <t>2016-04-29</t>
-  </si>
-  <si>
-    <t>2016-04-28</t>
-  </si>
-  <si>
-    <t>2016-04-27</t>
-  </si>
-  <si>
-    <t>2016-04-26</t>
-  </si>
-  <si>
-    <t>2016-04-25</t>
-  </si>
-  <si>
-    <t>2016-04-22</t>
-  </si>
-  <si>
-    <t>2016-04-21</t>
-  </si>
-  <si>
-    <t>2016-04-20</t>
-  </si>
-  <si>
-    <t>2016-04-19</t>
-  </si>
-  <si>
-    <t>2016-04-18</t>
-  </si>
-  <si>
-    <t>2016-04-15</t>
-  </si>
-  <si>
-    <t>2016-04-14</t>
-  </si>
-  <si>
-    <t>2016-04-13</t>
-  </si>
-  <si>
-    <t>2016-04-12</t>
-  </si>
-  <si>
-    <t>2016-04-11</t>
-  </si>
-  <si>
-    <t>2016-04-08</t>
-  </si>
-  <si>
-    <t>2016-04-07</t>
-  </si>
-  <si>
-    <t>2016-04-06</t>
-  </si>
-  <si>
-    <t>2016-04-05</t>
-  </si>
-  <si>
-    <t>2016-04-04</t>
-  </si>
-  <si>
-    <t>2016-04-01</t>
-  </si>
-  <si>
-    <t>2016-03-31</t>
-  </si>
-  <si>
-    <t>2016-03-30</t>
-  </si>
-  <si>
-    <t>2016-03-29</t>
-  </si>
-  <si>
-    <t>2016-03-28</t>
-  </si>
-  <si>
-    <t>2016-03-24</t>
-  </si>
-  <si>
-    <t>2016-03-23</t>
-  </si>
-  <si>
-    <t>2016-03-22</t>
-  </si>
-  <si>
-    <t>2016-03-21</t>
-  </si>
-  <si>
-    <t>2016-03-18</t>
-  </si>
-  <si>
-    <t>2016-03-17</t>
-  </si>
-  <si>
-    <t>2016-03-16</t>
-  </si>
-  <si>
-    <t>2016-03-15</t>
-  </si>
-  <si>
-    <t>2016-03-14</t>
-  </si>
-  <si>
-    <t>2016-03-11</t>
-  </si>
-  <si>
-    <t>2016-03-10</t>
-  </si>
-  <si>
-    <t>2016-03-09</t>
-  </si>
-  <si>
-    <t>2016-03-08</t>
-  </si>
-  <si>
-    <t>2016-03-07</t>
-  </si>
-  <si>
-    <t>2016-03-04</t>
-  </si>
-  <si>
-    <t>2016-03-03</t>
-  </si>
-  <si>
-    <t>2016-03-02</t>
-  </si>
-  <si>
-    <t>2016-03-01</t>
-  </si>
-  <si>
-    <t>2016-02-29</t>
-  </si>
-  <si>
-    <t>2016-02-26</t>
-  </si>
-  <si>
-    <t>2016-02-25</t>
-  </si>
-  <si>
-    <t>2016-02-24</t>
-  </si>
-  <si>
-    <t>2016-02-23</t>
-  </si>
-  <si>
-    <t>2016-02-22</t>
-  </si>
-  <si>
-    <t>2016-02-19</t>
-  </si>
-  <si>
-    <t>2016-02-18</t>
-  </si>
-  <si>
-    <t>2016-02-17</t>
-  </si>
-  <si>
-    <t>2016-02-16</t>
-  </si>
-  <si>
-    <t>2016-02-12</t>
-  </si>
-  <si>
-    <t>2016-02-11</t>
-  </si>
-  <si>
-    <t>2016-02-10</t>
-  </si>
-  <si>
-    <t>2016-02-09</t>
-  </si>
-  <si>
-    <t>2016-02-08</t>
-  </si>
-  <si>
-    <t>2016-02-05</t>
-  </si>
-  <si>
-    <t>2016-02-04</t>
-  </si>
-  <si>
-    <t>2016-02-03</t>
-  </si>
-  <si>
-    <t>2016-02-02</t>
-  </si>
-  <si>
-    <t>2016-02-01</t>
-  </si>
-  <si>
-    <t>2016-01-29</t>
-  </si>
-  <si>
-    <t>2016-01-28</t>
-  </si>
-  <si>
-    <t>2016-01-27</t>
-  </si>
-  <si>
-    <t>2016-01-26</t>
-  </si>
-  <si>
-    <t>2016-01-25</t>
-  </si>
-  <si>
-    <t>2016-01-22</t>
-  </si>
-  <si>
-    <t>2016-01-21</t>
-  </si>
-  <si>
-    <t>2016-01-20</t>
-  </si>
-  <si>
-    <t>2016-01-19</t>
-  </si>
-  <si>
-    <t>2016-01-15</t>
-  </si>
-  <si>
-    <t>2016-01-14</t>
-  </si>
-  <si>
-    <t>2016-01-13</t>
-  </si>
-  <si>
-    <t>2016-01-12</t>
-  </si>
-  <si>
-    <t>2016-01-11</t>
-  </si>
-  <si>
-    <t>2016-01-08</t>
-  </si>
-  <si>
-    <t>2016-01-07</t>
-  </si>
-  <si>
-    <t>2016-01-06</t>
-  </si>
-  <si>
-    <t>2016-01-05</t>
-  </si>
-  <si>
-    <t>2016-01-04</t>
+    <t>2014-12-31</t>
+  </si>
+  <si>
+    <t>2014-12-30</t>
+  </si>
+  <si>
+    <t>2014-12-29</t>
+  </si>
+  <si>
+    <t>2014-12-26</t>
+  </si>
+  <si>
+    <t>2014-12-24</t>
+  </si>
+  <si>
+    <t>2014-12-23</t>
+  </si>
+  <si>
+    <t>2014-12-22</t>
+  </si>
+  <si>
+    <t>2014-12-19</t>
+  </si>
+  <si>
+    <t>2014-12-18</t>
+  </si>
+  <si>
+    <t>2014-12-17</t>
+  </si>
+  <si>
+    <t>2014-12-16</t>
+  </si>
+  <si>
+    <t>2014-12-15</t>
+  </si>
+  <si>
+    <t>2014-12-12</t>
+  </si>
+  <si>
+    <t>2014-12-11</t>
+  </si>
+  <si>
+    <t>2014-12-10</t>
+  </si>
+  <si>
+    <t>2014-12-09</t>
+  </si>
+  <si>
+    <t>2014-12-08</t>
+  </si>
+  <si>
+    <t>2014-12-05</t>
+  </si>
+  <si>
+    <t>2014-12-04</t>
+  </si>
+  <si>
+    <t>2014-12-03</t>
+  </si>
+  <si>
+    <t>2014-12-02</t>
+  </si>
+  <si>
+    <t>2014-12-01</t>
+  </si>
+  <si>
+    <t>2014-11-28</t>
+  </si>
+  <si>
+    <t>2014-11-26</t>
+  </si>
+  <si>
+    <t>2014-11-25</t>
+  </si>
+  <si>
+    <t>2014-11-24</t>
+  </si>
+  <si>
+    <t>2014-11-21</t>
+  </si>
+  <si>
+    <t>2014-11-20</t>
+  </si>
+  <si>
+    <t>2014-11-19</t>
+  </si>
+  <si>
+    <t>2014-11-18</t>
+  </si>
+  <si>
+    <t>2014-11-17</t>
+  </si>
+  <si>
+    <t>2014-11-14</t>
+  </si>
+  <si>
+    <t>2014-11-13</t>
+  </si>
+  <si>
+    <t>2014-11-12</t>
+  </si>
+  <si>
+    <t>2014-11-10</t>
+  </si>
+  <si>
+    <t>2014-11-07</t>
+  </si>
+  <si>
+    <t>2014-11-06</t>
+  </si>
+  <si>
+    <t>2014-11-05</t>
+  </si>
+  <si>
+    <t>2014-11-04</t>
+  </si>
+  <si>
+    <t>2014-11-03</t>
+  </si>
+  <si>
+    <t>2014-10-31</t>
+  </si>
+  <si>
+    <t>2014-10-30</t>
+  </si>
+  <si>
+    <t>2014-10-29</t>
+  </si>
+  <si>
+    <t>2014-10-28</t>
+  </si>
+  <si>
+    <t>2014-10-27</t>
+  </si>
+  <si>
+    <t>2014-10-24</t>
+  </si>
+  <si>
+    <t>2014-10-23</t>
+  </si>
+  <si>
+    <t>2014-10-22</t>
+  </si>
+  <si>
+    <t>2014-10-21</t>
+  </si>
+  <si>
+    <t>2014-10-20</t>
+  </si>
+  <si>
+    <t>2014-10-17</t>
+  </si>
+  <si>
+    <t>2014-10-16</t>
+  </si>
+  <si>
+    <t>2014-10-15</t>
+  </si>
+  <si>
+    <t>2014-10-14</t>
+  </si>
+  <si>
+    <t>2014-10-10</t>
+  </si>
+  <si>
+    <t>2014-10-09</t>
+  </si>
+  <si>
+    <t>2014-10-08</t>
+  </si>
+  <si>
+    <t>2014-10-07</t>
+  </si>
+  <si>
+    <t>2014-10-06</t>
+  </si>
+  <si>
+    <t>2014-10-03</t>
+  </si>
+  <si>
+    <t>2014-10-02</t>
+  </si>
+  <si>
+    <t>2014-10-01</t>
+  </si>
+  <si>
+    <t>2014-09-30</t>
+  </si>
+  <si>
+    <t>2014-09-29</t>
+  </si>
+  <si>
+    <t>2014-09-26</t>
+  </si>
+  <si>
+    <t>2014-09-25</t>
+  </si>
+  <si>
+    <t>2014-09-24</t>
+  </si>
+  <si>
+    <t>2014-09-23</t>
+  </si>
+  <si>
+    <t>2014-09-22</t>
+  </si>
+  <si>
+    <t>2014-09-19</t>
+  </si>
+  <si>
+    <t>2014-09-18</t>
+  </si>
+  <si>
+    <t>2014-09-17</t>
+  </si>
+  <si>
+    <t>2014-09-16</t>
+  </si>
+  <si>
+    <t>2014-09-15</t>
+  </si>
+  <si>
+    <t>2014-09-12</t>
+  </si>
+  <si>
+    <t>2014-09-11</t>
+  </si>
+  <si>
+    <t>2014-09-10</t>
+  </si>
+  <si>
+    <t>2014-09-09</t>
+  </si>
+  <si>
+    <t>2014-09-08</t>
+  </si>
+  <si>
+    <t>2014-09-05</t>
+  </si>
+  <si>
+    <t>2014-09-04</t>
+  </si>
+  <si>
+    <t>2014-09-03</t>
+  </si>
+  <si>
+    <t>2014-09-02</t>
+  </si>
+  <si>
+    <t>2014-08-29</t>
+  </si>
+  <si>
+    <t>2014-08-28</t>
+  </si>
+  <si>
+    <t>2014-08-27</t>
+  </si>
+  <si>
+    <t>2014-08-26</t>
+  </si>
+  <si>
+    <t>2014-08-25</t>
+  </si>
+  <si>
+    <t>2014-08-22</t>
+  </si>
+  <si>
+    <t>2014-08-21</t>
+  </si>
+  <si>
+    <t>2014-08-20</t>
+  </si>
+  <si>
+    <t>2014-08-19</t>
+  </si>
+  <si>
+    <t>2014-08-18</t>
+  </si>
+  <si>
+    <t>2014-08-15</t>
+  </si>
+  <si>
+    <t>2014-08-14</t>
+  </si>
+  <si>
+    <t>2014-08-13</t>
+  </si>
+  <si>
+    <t>2014-08-12</t>
+  </si>
+  <si>
+    <t>2014-08-11</t>
+  </si>
+  <si>
+    <t>2014-08-08</t>
+  </si>
+  <si>
+    <t>2014-08-07</t>
+  </si>
+  <si>
+    <t>2014-08-06</t>
+  </si>
+  <si>
+    <t>2014-08-05</t>
+  </si>
+  <si>
+    <t>2014-08-04</t>
+  </si>
+  <si>
+    <t>2014-08-01</t>
+  </si>
+  <si>
+    <t>2014-07-31</t>
+  </si>
+  <si>
+    <t>2014-07-30</t>
+  </si>
+  <si>
+    <t>2014-07-29</t>
+  </si>
+  <si>
+    <t>2014-07-28</t>
+  </si>
+  <si>
+    <t>2014-07-25</t>
+  </si>
+  <si>
+    <t>2014-07-24</t>
+  </si>
+  <si>
+    <t>2014-07-23</t>
+  </si>
+  <si>
+    <t>2014-07-22</t>
+  </si>
+  <si>
+    <t>2014-07-21</t>
+  </si>
+  <si>
+    <t>2014-07-18</t>
+  </si>
+  <si>
+    <t>2014-07-17</t>
+  </si>
+  <si>
+    <t>2014-07-16</t>
+  </si>
+  <si>
+    <t>2014-07-15</t>
+  </si>
+  <si>
+    <t>2014-07-14</t>
+  </si>
+  <si>
+    <t>2014-07-11</t>
+  </si>
+  <si>
+    <t>2014-07-10</t>
+  </si>
+  <si>
+    <t>2014-07-09</t>
+  </si>
+  <si>
+    <t>2014-07-08</t>
+  </si>
+  <si>
+    <t>2014-07-07</t>
+  </si>
+  <si>
+    <t>2014-07-03</t>
+  </si>
+  <si>
+    <t>2014-07-02</t>
+  </si>
+  <si>
+    <t>2014-07-01</t>
+  </si>
+  <si>
+    <t>2014-06-30</t>
+  </si>
+  <si>
+    <t>2014-06-27</t>
+  </si>
+  <si>
+    <t>2014-06-26</t>
+  </si>
+  <si>
+    <t>2014-06-25</t>
+  </si>
+  <si>
+    <t>2014-06-24</t>
+  </si>
+  <si>
+    <t>2014-06-23</t>
+  </si>
+  <si>
+    <t>2014-06-20</t>
+  </si>
+  <si>
+    <t>2014-06-19</t>
+  </si>
+  <si>
+    <t>2014-06-18</t>
+  </si>
+  <si>
+    <t>2014-06-17</t>
+  </si>
+  <si>
+    <t>2014-06-16</t>
+  </si>
+  <si>
+    <t>2014-06-13</t>
+  </si>
+  <si>
+    <t>2014-06-12</t>
+  </si>
+  <si>
+    <t>2014-06-11</t>
+  </si>
+  <si>
+    <t>2014-06-10</t>
+  </si>
+  <si>
+    <t>2014-06-09</t>
+  </si>
+  <si>
+    <t>2014-06-06</t>
+  </si>
+  <si>
+    <t>2014-06-05</t>
+  </si>
+  <si>
+    <t>2014-06-04</t>
+  </si>
+  <si>
+    <t>2014-06-03</t>
+  </si>
+  <si>
+    <t>2014-06-02</t>
+  </si>
+  <si>
+    <t>2014-05-30</t>
+  </si>
+  <si>
+    <t>2014-05-29</t>
+  </si>
+  <si>
+    <t>2014-05-28</t>
+  </si>
+  <si>
+    <t>2014-05-27</t>
+  </si>
+  <si>
+    <t>2014-05-23</t>
+  </si>
+  <si>
+    <t>2014-05-22</t>
+  </si>
+  <si>
+    <t>2014-05-21</t>
+  </si>
+  <si>
+    <t>2014-05-20</t>
+  </si>
+  <si>
+    <t>2014-05-19</t>
+  </si>
+  <si>
+    <t>2014-05-16</t>
+  </si>
+  <si>
+    <t>2014-05-15</t>
+  </si>
+  <si>
+    <t>2014-05-14</t>
+  </si>
+  <si>
+    <t>2014-05-13</t>
+  </si>
+  <si>
+    <t>2014-05-12</t>
+  </si>
+  <si>
+    <t>2014-05-09</t>
+  </si>
+  <si>
+    <t>2014-05-08</t>
+  </si>
+  <si>
+    <t>2014-05-07</t>
+  </si>
+  <si>
+    <t>2014-05-06</t>
+  </si>
+  <si>
+    <t>2014-05-05</t>
+  </si>
+  <si>
+    <t>2014-05-02</t>
+  </si>
+  <si>
+    <t>2014-05-01</t>
+  </si>
+  <si>
+    <t>2014-04-30</t>
+  </si>
+  <si>
+    <t>2014-04-29</t>
+  </si>
+  <si>
+    <t>2014-04-28</t>
+  </si>
+  <si>
+    <t>2014-04-25</t>
+  </si>
+  <si>
+    <t>2014-04-24</t>
+  </si>
+  <si>
+    <t>2014-04-23</t>
+  </si>
+  <si>
+    <t>2014-04-22</t>
+  </si>
+  <si>
+    <t>2014-04-21</t>
+  </si>
+  <si>
+    <t>2014-04-17</t>
+  </si>
+  <si>
+    <t>2014-04-16</t>
+  </si>
+  <si>
+    <t>2014-04-15</t>
+  </si>
+  <si>
+    <t>2014-04-14</t>
+  </si>
+  <si>
+    <t>2014-04-11</t>
+  </si>
+  <si>
+    <t>2014-04-10</t>
+  </si>
+  <si>
+    <t>2014-04-09</t>
+  </si>
+  <si>
+    <t>2014-04-08</t>
+  </si>
+  <si>
+    <t>2014-04-07</t>
+  </si>
+  <si>
+    <t>2014-04-04</t>
+  </si>
+  <si>
+    <t>2014-04-03</t>
+  </si>
+  <si>
+    <t>2014-04-02</t>
+  </si>
+  <si>
+    <t>2014-04-01</t>
+  </si>
+  <si>
+    <t>2014-03-31</t>
+  </si>
+  <si>
+    <t>2014-03-28</t>
+  </si>
+  <si>
+    <t>2014-03-27</t>
+  </si>
+  <si>
+    <t>2014-03-26</t>
+  </si>
+  <si>
+    <t>2014-03-25</t>
+  </si>
+  <si>
+    <t>2014-03-24</t>
+  </si>
+  <si>
+    <t>2014-03-21</t>
+  </si>
+  <si>
+    <t>2014-03-20</t>
+  </si>
+  <si>
+    <t>2014-03-19</t>
+  </si>
+  <si>
+    <t>2014-03-18</t>
+  </si>
+  <si>
+    <t>2014-03-17</t>
+  </si>
+  <si>
+    <t>2014-03-14</t>
+  </si>
+  <si>
+    <t>2014-03-13</t>
+  </si>
+  <si>
+    <t>2014-03-12</t>
+  </si>
+  <si>
+    <t>2014-03-11</t>
+  </si>
+  <si>
+    <t>2014-03-10</t>
+  </si>
+  <si>
+    <t>2014-03-07</t>
+  </si>
+  <si>
+    <t>2014-03-06</t>
+  </si>
+  <si>
+    <t>2014-03-05</t>
+  </si>
+  <si>
+    <t>2014-03-04</t>
+  </si>
+  <si>
+    <t>2014-03-03</t>
+  </si>
+  <si>
+    <t>2014-02-28</t>
+  </si>
+  <si>
+    <t>2014-02-27</t>
+  </si>
+  <si>
+    <t>2014-02-26</t>
+  </si>
+  <si>
+    <t>2014-02-25</t>
+  </si>
+  <si>
+    <t>2014-02-24</t>
+  </si>
+  <si>
+    <t>2014-02-21</t>
+  </si>
+  <si>
+    <t>2014-02-20</t>
+  </si>
+  <si>
+    <t>2014-02-19</t>
+  </si>
+  <si>
+    <t>2014-02-18</t>
+  </si>
+  <si>
+    <t>2014-02-14</t>
+  </si>
+  <si>
+    <t>2014-02-13</t>
+  </si>
+  <si>
+    <t>2014-02-12</t>
+  </si>
+  <si>
+    <t>2014-02-11</t>
+  </si>
+  <si>
+    <t>2014-02-10</t>
+  </si>
+  <si>
+    <t>2014-02-07</t>
+  </si>
+  <si>
+    <t>2014-02-06</t>
+  </si>
+  <si>
+    <t>2014-02-05</t>
+  </si>
+  <si>
+    <t>2014-02-04</t>
+  </si>
+  <si>
+    <t>2014-02-03</t>
+  </si>
+  <si>
+    <t>2014-01-31</t>
+  </si>
+  <si>
+    <t>2014-01-30</t>
+  </si>
+  <si>
+    <t>2014-01-29</t>
+  </si>
+  <si>
+    <t>2014-01-28</t>
+  </si>
+  <si>
+    <t>2014-01-27</t>
+  </si>
+  <si>
+    <t>2014-01-24</t>
+  </si>
+  <si>
+    <t>2014-01-23</t>
+  </si>
+  <si>
+    <t>2014-01-22</t>
+  </si>
+  <si>
+    <t>2014-01-21</t>
+  </si>
+  <si>
+    <t>2014-01-17</t>
+  </si>
+  <si>
+    <t>2014-01-16</t>
+  </si>
+  <si>
+    <t>2014-01-15</t>
+  </si>
+  <si>
+    <t>2014-01-14</t>
+  </si>
+  <si>
+    <t>2014-01-13</t>
+  </si>
+  <si>
+    <t>2014-01-10</t>
+  </si>
+  <si>
+    <t>2014-01-09</t>
+  </si>
+  <si>
+    <t>2014-01-08</t>
+  </si>
+  <si>
+    <t>2014-01-07</t>
+  </si>
+  <si>
+    <t>2014-01-06</t>
+  </si>
+  <si>
+    <t>2014-01-03</t>
+  </si>
+  <si>
+    <t>2014-01-02</t>
   </si>
 </sst>
 </file>
@@ -1152,10 +1152,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2.91</v>
+        <v>2.55</v>
       </c>
       <c r="C2">
-        <v>2.79</v>
+        <v>2.47</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1163,10 +1163,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>2.94</v>
+        <v>2.56</v>
       </c>
       <c r="C3">
-        <v>2.82</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1174,10 +1174,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>2.95</v>
+        <v>2.58</v>
       </c>
       <c r="C4">
-        <v>2.83</v>
+        <v>2.51</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1185,10 +1185,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3.01</v>
+        <v>2.62</v>
       </c>
       <c r="C5">
-        <v>2.88</v>
+        <v>2.54</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1196,10 +1196,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>2.98</v>
+        <v>2.63</v>
       </c>
       <c r="C6">
-        <v>2.86</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1207,10 +1207,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>2.99</v>
+        <v>2.64</v>
       </c>
       <c r="C7">
-        <v>2.86</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1218,10 +1218,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>2.98</v>
+        <v>2.55</v>
       </c>
       <c r="C8">
-        <v>2.86</v>
+        <v>2.47</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1229,10 +1229,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>3.01</v>
+        <v>2.56</v>
       </c>
       <c r="C9">
-        <v>2.88</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1240,10 +1240,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>2.97</v>
+        <v>2.61</v>
       </c>
       <c r="C10">
-        <v>2.85</v>
+        <v>2.54</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1251,10 +1251,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>3.04</v>
+        <v>2.53</v>
       </c>
       <c r="C11">
-        <v>2.91</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1262,10 +1262,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>3.02</v>
+        <v>2.48</v>
       </c>
       <c r="C12">
-        <v>2.89</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1273,10 +1273,10 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>2.99</v>
+        <v>2.53</v>
       </c>
       <c r="C13">
-        <v>2.86</v>
+        <v>2.45</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1284,10 +1284,10 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>2.97</v>
+        <v>2.53</v>
       </c>
       <c r="C14">
-        <v>2.85</v>
+        <v>2.45</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1295,10 +1295,10 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>2.99</v>
+        <v>2.62</v>
       </c>
       <c r="C15">
-        <v>2.86</v>
+        <v>2.54</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1306,10 +1306,10 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>2.99</v>
+        <v>2.61</v>
       </c>
       <c r="C16">
-        <v>2.87</v>
+        <v>2.54</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1317,10 +1317,10 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>2.93</v>
+        <v>2.65</v>
       </c>
       <c r="C17">
-        <v>2.81</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1328,10 +1328,10 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>2.85</v>
+        <v>2.69</v>
       </c>
       <c r="C18">
-        <v>2.73</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1339,10 +1339,10 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>2.9</v>
+        <v>2.75</v>
       </c>
       <c r="C19">
-        <v>2.77</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1350,10 +1350,10 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>2.89</v>
+        <v>2.72</v>
       </c>
       <c r="C20">
-        <v>2.76</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1361,10 +1361,10 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>2.91</v>
+        <v>2.76</v>
       </c>
       <c r="C21">
-        <v>2.78</v>
+        <v>2.71</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1372,10 +1372,10 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>2.94</v>
+        <v>2.77</v>
       </c>
       <c r="C22">
-        <v>2.82</v>
+        <v>2.72</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1383,10 +1383,10 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>2.86</v>
+        <v>2.72</v>
       </c>
       <c r="C23">
-        <v>2.73</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1394,10 +1394,10 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>2.79</v>
+        <v>2.67</v>
       </c>
       <c r="C24">
-        <v>2.66</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1405,10 +1405,10 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>2.82</v>
+        <v>2.73</v>
       </c>
       <c r="C25">
-        <v>2.68</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1416,10 +1416,10 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>2.84</v>
+        <v>2.75</v>
       </c>
       <c r="C26">
-        <v>2.71</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1427,10 +1427,10 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>2.85</v>
+        <v>2.79</v>
       </c>
       <c r="C27">
-        <v>2.71</v>
+        <v>2.74</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1438,10 +1438,10 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>2.83</v>
+        <v>2.8</v>
       </c>
       <c r="C28">
-        <v>2.69</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1452,7 +1452,7 @@
         <v>2.83</v>
       </c>
       <c r="C29">
-        <v>2.69</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1460,10 +1460,10 @@
         <v>31</v>
       </c>
       <c r="B30">
-        <v>2.84</v>
+        <v>2.85</v>
       </c>
       <c r="C30">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1471,10 +1471,10 @@
         <v>32</v>
       </c>
       <c r="B31">
-        <v>2.82</v>
+        <v>2.83</v>
       </c>
       <c r="C31">
-        <v>2.69</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1482,10 +1482,10 @@
         <v>33</v>
       </c>
       <c r="B32">
-        <v>2.74</v>
+        <v>2.84</v>
       </c>
       <c r="C32">
-        <v>2.61</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1493,10 +1493,10 @@
         <v>34</v>
       </c>
       <c r="B33">
-        <v>2.76</v>
+        <v>2.8</v>
       </c>
       <c r="C33">
-        <v>2.64</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1504,10 +1504,10 @@
         <v>35</v>
       </c>
       <c r="B34">
-        <v>2.77</v>
+        <v>2.83</v>
       </c>
       <c r="C34">
-        <v>2.65</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1515,10 +1515,10 @@
         <v>36</v>
       </c>
       <c r="B35">
-        <v>2.71</v>
+        <v>2.84</v>
       </c>
       <c r="C35">
-        <v>2.58</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1526,10 +1526,10 @@
         <v>37</v>
       </c>
       <c r="B36">
-        <v>2.63</v>
+        <v>2.85</v>
       </c>
       <c r="C36">
-        <v>2.52</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1537,10 +1537,10 @@
         <v>38</v>
       </c>
       <c r="B37">
-        <v>2.4</v>
+        <v>2.79</v>
       </c>
       <c r="C37">
-        <v>2.29</v>
+        <v>2.76</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1548,10 +1548,10 @@
         <v>39</v>
       </c>
       <c r="B38">
-        <v>2.36</v>
+        <v>2.86</v>
       </c>
       <c r="C38">
-        <v>2.26</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1559,10 +1559,10 @@
         <v>40</v>
       </c>
       <c r="B39">
-        <v>2.33</v>
+        <v>2.82</v>
       </c>
       <c r="C39">
-        <v>2.22</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1570,10 +1570,10 @@
         <v>41</v>
       </c>
       <c r="B40">
-        <v>2.36</v>
+        <v>2.81</v>
       </c>
       <c r="C40">
-        <v>2.25</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1581,10 +1581,10 @@
         <v>42</v>
       </c>
       <c r="B41">
-        <v>2.33</v>
+        <v>2.83</v>
       </c>
       <c r="C41">
-        <v>2.22</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1592,10 +1592,10 @@
         <v>43</v>
       </c>
       <c r="B42">
-        <v>2.35</v>
+        <v>2.83</v>
       </c>
       <c r="C42">
-        <v>2.24</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1603,10 +1603,10 @@
         <v>44</v>
       </c>
       <c r="B43">
-        <v>2.36</v>
+        <v>2.8</v>
       </c>
       <c r="C43">
-        <v>2.25</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1614,10 +1614,10 @@
         <v>45</v>
       </c>
       <c r="B44">
-        <v>2.38</v>
+        <v>2.82</v>
       </c>
       <c r="C44">
-        <v>2.27</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1625,10 +1625,10 @@
         <v>46</v>
       </c>
       <c r="B45">
-        <v>2.37</v>
+        <v>2.81</v>
       </c>
       <c r="C45">
-        <v>2.26</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1636,10 +1636,10 @@
         <v>47</v>
       </c>
       <c r="B46">
-        <v>2.31</v>
+        <v>2.78</v>
       </c>
       <c r="C46">
-        <v>2.2</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1647,10 +1647,10 @@
         <v>48</v>
       </c>
       <c r="B47">
-        <v>2.28</v>
+        <v>2.79</v>
       </c>
       <c r="C47">
-        <v>2.17</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1658,10 +1658,10 @@
         <v>49</v>
       </c>
       <c r="B48">
-        <v>2.29</v>
+        <v>2.79</v>
       </c>
       <c r="C48">
-        <v>2.18</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1669,10 +1669,10 @@
         <v>50</v>
       </c>
       <c r="B49">
-        <v>2.26</v>
+        <v>2.75</v>
       </c>
       <c r="C49">
-        <v>2.15</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1680,10 +1680,10 @@
         <v>51</v>
       </c>
       <c r="B50">
-        <v>2.28</v>
+        <v>2.74</v>
       </c>
       <c r="C50">
-        <v>2.17</v>
+        <v>2.72</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1691,10 +1691,10 @@
         <v>52</v>
       </c>
       <c r="B51">
-        <v>2.29</v>
+        <v>2.7</v>
       </c>
       <c r="C51">
-        <v>2.18</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1702,10 +1702,10 @@
         <v>53</v>
       </c>
       <c r="B52">
-        <v>2.28</v>
+        <v>2.73</v>
       </c>
       <c r="C52">
-        <v>2.18</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1713,10 +1713,10 @@
         <v>54</v>
       </c>
       <c r="B53">
-        <v>2.29</v>
+        <v>2.68</v>
       </c>
       <c r="C53">
-        <v>2.19</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1724,10 +1724,10 @@
         <v>55</v>
       </c>
       <c r="B54">
-        <v>2.33</v>
+        <v>2.66</v>
       </c>
       <c r="C54">
-        <v>2.22</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1735,10 +1735,10 @@
         <v>56</v>
       </c>
       <c r="B55">
-        <v>2.26</v>
+        <v>2.7</v>
       </c>
       <c r="C55">
-        <v>2.15</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1746,10 +1746,10 @@
         <v>57</v>
       </c>
       <c r="B56">
-        <v>2.29</v>
+        <v>2.79</v>
       </c>
       <c r="C56">
-        <v>2.19</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1757,10 +1757,10 @@
         <v>58</v>
       </c>
       <c r="B57">
-        <v>2.28</v>
+        <v>2.82</v>
       </c>
       <c r="C57">
-        <v>2.17</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1768,10 +1768,10 @@
         <v>59</v>
       </c>
       <c r="B58">
-        <v>2.24</v>
+        <v>2.83</v>
       </c>
       <c r="C58">
-        <v>2.14</v>
+        <v>2.82</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1779,10 +1779,10 @@
         <v>60</v>
       </c>
       <c r="B59">
-        <v>2.25</v>
+        <v>2.82</v>
       </c>
       <c r="C59">
-        <v>2.14</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1790,10 +1790,10 @@
         <v>61</v>
       </c>
       <c r="B60">
-        <v>2.22</v>
+        <v>2.89</v>
       </c>
       <c r="C60">
-        <v>2.11</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1801,10 +1801,10 @@
         <v>62</v>
       </c>
       <c r="B61">
-        <v>2.18</v>
+        <v>2.9</v>
       </c>
       <c r="C61">
-        <v>2.08</v>
+        <v>2.89</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1812,10 +1812,10 @@
         <v>63</v>
       </c>
       <c r="B62">
-        <v>2.12</v>
+        <v>2.91</v>
       </c>
       <c r="C62">
-        <v>2.01</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1823,10 +1823,10 @@
         <v>64</v>
       </c>
       <c r="B63">
-        <v>2.1</v>
+        <v>2.88</v>
       </c>
       <c r="C63">
-        <v>1.99</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1834,10 +1834,10 @@
         <v>65</v>
       </c>
       <c r="B64">
-        <v>2.06</v>
+        <v>2.98</v>
       </c>
       <c r="C64">
-        <v>1.95</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1845,10 +1845,10 @@
         <v>66</v>
       </c>
       <c r="B65">
-        <v>2.07</v>
+        <v>2.95</v>
       </c>
       <c r="C65">
-        <v>1.96</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1856,10 +1856,10 @@
         <v>67</v>
       </c>
       <c r="B66">
-        <v>2.06</v>
+        <v>2.99</v>
       </c>
       <c r="C66">
-        <v>1.96</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1867,10 +1867,10 @@
         <v>68</v>
       </c>
       <c r="B67">
-        <v>2.1</v>
+        <v>2.98</v>
       </c>
       <c r="C67">
-        <v>2</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1878,10 +1878,10 @@
         <v>69</v>
       </c>
       <c r="B68">
-        <v>2.12</v>
+        <v>3.04</v>
       </c>
       <c r="C68">
-        <v>2.02</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1889,10 +1889,10 @@
         <v>70</v>
       </c>
       <c r="B69">
-        <v>2.13</v>
+        <v>3.01</v>
       </c>
       <c r="C69">
-        <v>2.02</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1900,10 +1900,10 @@
         <v>71</v>
       </c>
       <c r="B70">
-        <v>2.17</v>
+        <v>3.05</v>
       </c>
       <c r="C70">
-        <v>2.06</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1911,10 +1911,10 @@
         <v>72</v>
       </c>
       <c r="B71">
-        <v>2.2</v>
+        <v>3.06</v>
       </c>
       <c r="C71">
-        <v>2.09</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1922,10 +1922,10 @@
         <v>73</v>
       </c>
       <c r="B72">
-        <v>2.22</v>
+        <v>3.12</v>
       </c>
       <c r="C72">
-        <v>2.1</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1933,10 +1933,10 @@
         <v>74</v>
       </c>
       <c r="B73">
-        <v>2.21</v>
+        <v>3.13</v>
       </c>
       <c r="C73">
-        <v>2.1</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1944,10 +1944,10 @@
         <v>75</v>
       </c>
       <c r="B74">
-        <v>2.25</v>
+        <v>3.11</v>
       </c>
       <c r="C74">
-        <v>2.13</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1955,10 +1955,10 @@
         <v>76</v>
       </c>
       <c r="B75">
-        <v>2.21</v>
+        <v>3.1</v>
       </c>
       <c r="C75">
-        <v>2.1</v>
+        <v>3.09</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1966,10 +1966,10 @@
         <v>77</v>
       </c>
       <c r="B76">
-        <v>2.24</v>
+        <v>3.11</v>
       </c>
       <c r="C76">
-        <v>2.12</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1977,10 +1977,10 @@
         <v>78</v>
       </c>
       <c r="B77">
-        <v>2.17</v>
+        <v>3.03</v>
       </c>
       <c r="C77">
-        <v>2.05</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1988,10 +1988,10 @@
         <v>79</v>
       </c>
       <c r="B78">
-        <v>2.17</v>
+        <v>3.02</v>
       </c>
       <c r="C78">
-        <v>2.05</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1999,10 +1999,10 @@
         <v>80</v>
       </c>
       <c r="B79">
-        <v>2.09</v>
+        <v>2.98</v>
       </c>
       <c r="C79">
-        <v>1.98</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2010,10 +2010,10 @@
         <v>81</v>
       </c>
       <c r="B80">
-        <v>2.01</v>
+        <v>2.98</v>
       </c>
       <c r="C80">
-        <v>1.89</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2021,10 +2021,10 @@
         <v>82</v>
       </c>
       <c r="B81">
-        <v>2.02</v>
+        <v>2.98</v>
       </c>
       <c r="C81">
-        <v>1.9</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2032,10 +2032,10 @@
         <v>83</v>
       </c>
       <c r="B82">
-        <v>2.06</v>
+        <v>2.96</v>
       </c>
       <c r="C82">
-        <v>1.95</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2043,10 +2043,10 @@
         <v>84</v>
       </c>
       <c r="B83">
-        <v>2.02</v>
+        <v>2.91</v>
       </c>
       <c r="C83">
-        <v>1.9</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2054,10 +2054,10 @@
         <v>85</v>
       </c>
       <c r="B84">
-        <v>2.02</v>
+        <v>2.92</v>
       </c>
       <c r="C84">
-        <v>1.9</v>
+        <v>2.91</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2065,10 +2065,10 @@
         <v>86</v>
       </c>
       <c r="B85">
-        <v>2.03</v>
+        <v>2.84</v>
       </c>
       <c r="C85">
-        <v>1.91</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2076,10 +2076,10 @@
         <v>87</v>
       </c>
       <c r="B86">
-        <v>2.01</v>
+        <v>2.83</v>
       </c>
       <c r="C86">
-        <v>1.9</v>
+        <v>2.82</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2087,10 +2087,10 @@
         <v>88</v>
       </c>
       <c r="B87">
-        <v>2.08</v>
+        <v>2.86</v>
       </c>
       <c r="C87">
-        <v>1.96</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2098,10 +2098,10 @@
         <v>89</v>
       </c>
       <c r="B88">
-        <v>2.04</v>
+        <v>2.9</v>
       </c>
       <c r="C88">
-        <v>1.91</v>
+        <v>2.89</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2109,10 +2109,10 @@
         <v>90</v>
       </c>
       <c r="B89">
-        <v>2.02</v>
+        <v>2.89</v>
       </c>
       <c r="C89">
-        <v>1.89</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2120,10 +2120,10 @@
         <v>91</v>
       </c>
       <c r="B90">
-        <v>2.01</v>
+        <v>2.91</v>
       </c>
       <c r="C90">
-        <v>1.88</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2131,10 +2131,10 @@
         <v>92</v>
       </c>
       <c r="B91">
-        <v>2.02</v>
+        <v>2.93</v>
       </c>
       <c r="C91">
-        <v>1.88</v>
+        <v>2.92</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2142,10 +2142,10 @@
         <v>93</v>
       </c>
       <c r="B92">
-        <v>2.06</v>
+        <v>2.96</v>
       </c>
       <c r="C92">
-        <v>1.93</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2153,10 +2153,10 @@
         <v>94</v>
       </c>
       <c r="B93">
-        <v>2.02</v>
+        <v>2.95</v>
       </c>
       <c r="C93">
-        <v>1.89</v>
+        <v>2.94</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2164,10 +2164,10 @@
         <v>95</v>
       </c>
       <c r="B94">
-        <v>2.04</v>
+        <v>2.93</v>
       </c>
       <c r="C94">
-        <v>1.9</v>
+        <v>2.92</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2175,10 +2175,10 @@
         <v>96</v>
       </c>
       <c r="B95">
-        <v>2.06</v>
+        <v>2.87</v>
       </c>
       <c r="C95">
-        <v>1.92</v>
+        <v>2.86</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2186,10 +2186,10 @@
         <v>97</v>
       </c>
       <c r="B96">
-        <v>2.03</v>
+        <v>2.93</v>
       </c>
       <c r="C96">
-        <v>1.9</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2197,10 +2197,10 @@
         <v>98</v>
       </c>
       <c r="B97">
-        <v>1.98</v>
+        <v>2.98</v>
       </c>
       <c r="C97">
-        <v>1.85</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2208,10 +2208,10 @@
         <v>99</v>
       </c>
       <c r="B98">
-        <v>2.03</v>
+        <v>3.01</v>
       </c>
       <c r="C98">
-        <v>1.89</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2219,10 +2219,10 @@
         <v>100</v>
       </c>
       <c r="B99">
-        <v>1.97</v>
+        <v>2.98</v>
       </c>
       <c r="C99">
-        <v>1.83</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2230,10 +2230,10 @@
         <v>101</v>
       </c>
       <c r="B100">
-        <v>1.99</v>
+        <v>2.97</v>
       </c>
       <c r="C100">
-        <v>1.86</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2241,10 +2241,10 @@
         <v>102</v>
       </c>
       <c r="B101">
-        <v>2.04</v>
+        <v>2.97</v>
       </c>
       <c r="C101">
-        <v>1.91</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2252,10 +2252,10 @@
         <v>103</v>
       </c>
       <c r="B102">
-        <v>2.05</v>
+        <v>3.01</v>
       </c>
       <c r="C102">
-        <v>1.91</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2263,10 +2263,10 @@
         <v>104</v>
       </c>
       <c r="B103">
-        <v>1.98</v>
+        <v>3.02</v>
       </c>
       <c r="C103">
-        <v>1.84</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2274,10 +2274,10 @@
         <v>105</v>
       </c>
       <c r="B104">
-        <v>2.02</v>
+        <v>3.03</v>
       </c>
       <c r="C104">
-        <v>1.88</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2285,10 +2285,10 @@
         <v>106</v>
       </c>
       <c r="B105">
-        <v>2.02</v>
+        <v>3.03</v>
       </c>
       <c r="C105">
-        <v>1.88</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2296,10 +2296,10 @@
         <v>107</v>
       </c>
       <c r="B106">
-        <v>1.98</v>
+        <v>3.07</v>
       </c>
       <c r="C106">
-        <v>1.84</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2307,10 +2307,10 @@
         <v>108</v>
       </c>
       <c r="B107">
-        <v>1.92</v>
+        <v>3.06</v>
       </c>
       <c r="C107">
-        <v>1.78</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2318,10 +2318,10 @@
         <v>109</v>
       </c>
       <c r="B108">
-        <v>1.97</v>
+        <v>2.97</v>
       </c>
       <c r="C108">
-        <v>1.83</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2329,10 +2329,10 @@
         <v>110</v>
       </c>
       <c r="B109">
-        <v>1.97</v>
+        <v>3.01</v>
       </c>
       <c r="C109">
-        <v>1.84</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2340,10 +2340,10 @@
         <v>111</v>
       </c>
       <c r="B110">
-        <v>2.02</v>
+        <v>2.99</v>
       </c>
       <c r="C110">
-        <v>1.89</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2351,10 +2351,10 @@
         <v>112</v>
       </c>
       <c r="B111">
-        <v>2.03</v>
+        <v>3.04</v>
       </c>
       <c r="C111">
-        <v>1.9</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2362,10 +2362,10 @@
         <v>113</v>
       </c>
       <c r="B112">
-        <v>2.03</v>
+        <v>3</v>
       </c>
       <c r="C112">
-        <v>1.9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2373,10 +2373,10 @@
         <v>114</v>
       </c>
       <c r="B113">
-        <v>2.03</v>
+        <v>3</v>
       </c>
       <c r="C113">
-        <v>1.9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2384,10 +2384,10 @@
         <v>115</v>
       </c>
       <c r="B114">
-        <v>2.05</v>
+        <v>3</v>
       </c>
       <c r="C114">
-        <v>1.91</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2395,10 +2395,10 @@
         <v>116</v>
       </c>
       <c r="B115">
-        <v>2.02</v>
+        <v>3.03</v>
       </c>
       <c r="C115">
-        <v>1.88</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2406,10 +2406,10 @@
         <v>117</v>
       </c>
       <c r="B116">
-        <v>2.04</v>
+        <v>3.01</v>
       </c>
       <c r="C116">
-        <v>1.9</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2417,10 +2417,10 @@
         <v>118</v>
       </c>
       <c r="B117">
-        <v>2.04</v>
+        <v>3.08</v>
       </c>
       <c r="C117">
-        <v>1.9</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2428,10 +2428,10 @@
         <v>119</v>
       </c>
       <c r="B118">
-        <v>1.99</v>
+        <v>3.1</v>
       </c>
       <c r="C118">
-        <v>1.84</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2439,10 +2439,10 @@
         <v>120</v>
       </c>
       <c r="B119">
-        <v>1.92</v>
+        <v>3.1</v>
       </c>
       <c r="C119">
-        <v>1.77</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2450,10 +2450,10 @@
         <v>121</v>
       </c>
       <c r="B120">
-        <v>1.98</v>
+        <v>3.07</v>
       </c>
       <c r="C120">
-        <v>1.82</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2461,10 +2461,10 @@
         <v>122</v>
       </c>
       <c r="B121">
-        <v>1.88</v>
+        <v>3.1</v>
       </c>
       <c r="C121">
-        <v>1.73</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2472,10 +2472,10 @@
         <v>123</v>
       </c>
       <c r="B122">
-        <v>1.84</v>
+        <v>3.1</v>
       </c>
       <c r="C122">
-        <v>1.69</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2483,10 +2483,10 @@
         <v>124</v>
       </c>
       <c r="B123">
-        <v>1.87</v>
+        <v>3.12</v>
       </c>
       <c r="C123">
-        <v>1.72</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2494,10 +2494,10 @@
         <v>125</v>
       </c>
       <c r="B124">
-        <v>1.87</v>
+        <v>3.17</v>
       </c>
       <c r="C124">
-        <v>1.72</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2505,10 +2505,10 @@
         <v>126</v>
       </c>
       <c r="B125">
-        <v>1.86</v>
+        <v>3.2</v>
       </c>
       <c r="C125">
-        <v>1.72</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2516,10 +2516,10 @@
         <v>127</v>
       </c>
       <c r="B126">
-        <v>1.96</v>
+        <v>3.2</v>
       </c>
       <c r="C126">
-        <v>1.81</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2527,10 +2527,10 @@
         <v>128</v>
       </c>
       <c r="B127">
-        <v>2.01</v>
+        <v>3.13</v>
       </c>
       <c r="C127">
-        <v>1.86</v>
+        <v>3.13</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2538,10 +2538,10 @@
         <v>129</v>
       </c>
       <c r="B128">
-        <v>2.01</v>
+        <v>3.08</v>
       </c>
       <c r="C128">
-        <v>1.86</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2549,10 +2549,10 @@
         <v>130</v>
       </c>
       <c r="B129">
-        <v>1.98</v>
+        <v>3.09</v>
       </c>
       <c r="C129">
-        <v>1.83</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2560,10 +2560,10 @@
         <v>131</v>
       </c>
       <c r="B130">
-        <v>1.99</v>
+        <v>3.08</v>
       </c>
       <c r="C130">
-        <v>1.83</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2571,10 +2571,10 @@
         <v>132</v>
       </c>
       <c r="B131">
-        <v>2.12</v>
+        <v>3.12</v>
       </c>
       <c r="C131">
-        <v>1.96</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2582,10 +2582,10 @@
         <v>133</v>
       </c>
       <c r="B132">
-        <v>2.27</v>
+        <v>3.14</v>
       </c>
       <c r="C132">
-        <v>2.12</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2593,10 +2593,10 @@
         <v>134</v>
       </c>
       <c r="B133">
-        <v>2.21</v>
+        <v>3.18</v>
       </c>
       <c r="C133">
-        <v>2.06</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2604,10 +2604,10 @@
         <v>135</v>
       </c>
       <c r="B134">
-        <v>2.22</v>
+        <v>3.18</v>
       </c>
       <c r="C134">
-        <v>2.07</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2615,10 +2615,10 @@
         <v>136</v>
       </c>
       <c r="B135">
-        <v>2.18</v>
+        <v>3.2</v>
       </c>
       <c r="C135">
-        <v>2.03</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2626,10 +2626,10 @@
         <v>137</v>
       </c>
       <c r="B136">
-        <v>2.14</v>
+        <v>3.16</v>
       </c>
       <c r="C136">
-        <v>1.99</v>
+        <v>3.16</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2637,10 +2637,10 @@
         <v>138</v>
       </c>
       <c r="B137">
-        <v>2.1</v>
+        <v>3.18</v>
       </c>
       <c r="C137">
-        <v>1.96</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2648,10 +2648,10 @@
         <v>139</v>
       </c>
       <c r="B138">
-        <v>2.14</v>
+        <v>3.14</v>
       </c>
       <c r="C138">
-        <v>1.99</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2659,10 +2659,10 @@
         <v>140</v>
       </c>
       <c r="B139">
-        <v>2.15</v>
+        <v>3.14</v>
       </c>
       <c r="C139">
-        <v>2</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2670,10 +2670,10 @@
         <v>141</v>
       </c>
       <c r="B140">
-        <v>2.15</v>
+        <v>3.14</v>
       </c>
       <c r="C140">
-        <v>2.01</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2681,10 +2681,10 @@
         <v>142</v>
       </c>
       <c r="B141">
-        <v>2.16</v>
+        <v>3.2</v>
       </c>
       <c r="C141">
-        <v>2.02</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2692,10 +2692,10 @@
         <v>143</v>
       </c>
       <c r="B142">
-        <v>2.2</v>
+        <v>3.2</v>
       </c>
       <c r="C142">
-        <v>2.05</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2703,10 +2703,10 @@
         <v>144</v>
       </c>
       <c r="B143">
-        <v>2.23</v>
+        <v>3.17</v>
       </c>
       <c r="C143">
-        <v>2.08</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2714,10 +2714,10 @@
         <v>145</v>
       </c>
       <c r="B144">
-        <v>2.25</v>
+        <v>3.16</v>
       </c>
       <c r="C144">
-        <v>2.1</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2725,10 +2725,10 @@
         <v>146</v>
       </c>
       <c r="B145">
-        <v>2.27</v>
+        <v>3.16</v>
       </c>
       <c r="C145">
-        <v>2.12</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2736,10 +2736,10 @@
         <v>147</v>
       </c>
       <c r="B146">
-        <v>2.24</v>
+        <v>3.18</v>
       </c>
       <c r="C146">
-        <v>2.09</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2747,10 +2747,10 @@
         <v>148</v>
       </c>
       <c r="B147">
-        <v>2.32</v>
+        <v>3.16</v>
       </c>
       <c r="C147">
-        <v>2.17</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2758,10 +2758,10 @@
         <v>149</v>
       </c>
       <c r="B148">
-        <v>2.36</v>
+        <v>3.1</v>
       </c>
       <c r="C148">
-        <v>2.22</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2769,10 +2769,10 @@
         <v>150</v>
       </c>
       <c r="B149">
-        <v>2.37</v>
+        <v>3.05</v>
       </c>
       <c r="C149">
-        <v>2.23</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2780,10 +2780,10 @@
         <v>151</v>
       </c>
       <c r="B150">
-        <v>2.39</v>
+        <v>3.03</v>
       </c>
       <c r="C150">
-        <v>2.25</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2791,10 +2791,10 @@
         <v>152</v>
       </c>
       <c r="B151">
-        <v>2.37</v>
+        <v>3.01</v>
       </c>
       <c r="C151">
-        <v>2.24</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2802,10 +2802,10 @@
         <v>153</v>
       </c>
       <c r="B152">
-        <v>2.4</v>
+        <v>3.09</v>
       </c>
       <c r="C152">
-        <v>2.27</v>
+        <v>3.09</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2813,10 +2813,10 @@
         <v>154</v>
       </c>
       <c r="B153">
-        <v>2.39</v>
+        <v>3.12</v>
       </c>
       <c r="C153">
-        <v>2.25</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2824,10 +2824,10 @@
         <v>155</v>
       </c>
       <c r="B154">
-        <v>2.37</v>
+        <v>3.14</v>
       </c>
       <c r="C154">
-        <v>2.23</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2835,10 +2835,10 @@
         <v>156</v>
       </c>
       <c r="B155">
-        <v>2.37</v>
+        <v>3.13</v>
       </c>
       <c r="C155">
-        <v>2.24</v>
+        <v>3.13</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2846,10 +2846,10 @@
         <v>157</v>
       </c>
       <c r="B156">
-        <v>2.38</v>
+        <v>3.09</v>
       </c>
       <c r="C156">
-        <v>2.24</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2857,10 +2857,10 @@
         <v>158</v>
       </c>
       <c r="B157">
-        <v>2.41</v>
+        <v>3.1</v>
       </c>
       <c r="C157">
-        <v>2.27</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2868,10 +2868,10 @@
         <v>159</v>
       </c>
       <c r="B158">
-        <v>2.31</v>
+        <v>3.07</v>
       </c>
       <c r="C158">
-        <v>2.18</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2879,10 +2879,10 @@
         <v>160</v>
       </c>
       <c r="B159">
-        <v>2.32</v>
+        <v>3.05</v>
       </c>
       <c r="C159">
-        <v>2.18</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2890,10 +2890,10 @@
         <v>161</v>
       </c>
       <c r="B160">
-        <v>2.27</v>
+        <v>3.09</v>
       </c>
       <c r="C160">
-        <v>2.14</v>
+        <v>3.09</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2901,10 +2901,10 @@
         <v>162</v>
       </c>
       <c r="B161">
-        <v>2.32</v>
+        <v>3.16</v>
       </c>
       <c r="C161">
-        <v>2.18</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2912,10 +2912,10 @@
         <v>163</v>
       </c>
       <c r="B162">
-        <v>2.29</v>
+        <v>3.2</v>
       </c>
       <c r="C162">
-        <v>2.15</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2923,10 +2923,10 @@
         <v>164</v>
       </c>
       <c r="B163">
-        <v>2.32</v>
+        <v>3.18</v>
       </c>
       <c r="C163">
-        <v>2.18</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2934,10 +2934,10 @@
         <v>165</v>
       </c>
       <c r="B164">
-        <v>2.32</v>
+        <v>3.16</v>
       </c>
       <c r="C164">
-        <v>2.18</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2945,10 +2945,10 @@
         <v>166</v>
       </c>
       <c r="B165">
-        <v>2.33</v>
+        <v>3.14</v>
       </c>
       <c r="C165">
-        <v>2.2</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2956,10 +2956,10 @@
         <v>167</v>
       </c>
       <c r="B166">
-        <v>2.31</v>
+        <v>3.12</v>
       </c>
       <c r="C166">
-        <v>2.17</v>
+        <v>3.13</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2967,10 +2967,10 @@
         <v>168</v>
       </c>
       <c r="B167">
-        <v>2.35</v>
+        <v>3.15</v>
       </c>
       <c r="C167">
-        <v>2.22</v>
+        <v>3.16</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2978,10 +2978,10 @@
         <v>169</v>
       </c>
       <c r="B168">
-        <v>2.37</v>
+        <v>3.11</v>
       </c>
       <c r="C168">
-        <v>2.24</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2989,10 +2989,10 @@
         <v>170</v>
       </c>
       <c r="B169">
-        <v>2.44</v>
+        <v>3.15</v>
       </c>
       <c r="C169">
-        <v>2.31</v>
+        <v>3.16</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3000,10 +3000,10 @@
         <v>171</v>
       </c>
       <c r="B170">
-        <v>2.38</v>
+        <v>3.21</v>
       </c>
       <c r="C170">
-        <v>2.26</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3011,10 +3011,10 @@
         <v>172</v>
       </c>
       <c r="B171">
-        <v>2.4</v>
+        <v>3.24</v>
       </c>
       <c r="C171">
-        <v>2.27</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3022,10 +3022,10 @@
         <v>173</v>
       </c>
       <c r="B172">
-        <v>2.43</v>
+        <v>3.22</v>
       </c>
       <c r="C172">
-        <v>2.3</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3033,10 +3033,10 @@
         <v>174</v>
       </c>
       <c r="B173">
-        <v>2.49</v>
+        <v>3.2</v>
       </c>
       <c r="C173">
-        <v>2.35</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -3044,10 +3044,10 @@
         <v>175</v>
       </c>
       <c r="B174">
-        <v>2.45</v>
+        <v>3.21</v>
       </c>
       <c r="C174">
-        <v>2.32</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3055,10 +3055,10 @@
         <v>176</v>
       </c>
       <c r="B175">
-        <v>2.43</v>
+        <v>3.22</v>
       </c>
       <c r="C175">
-        <v>2.3</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -3066,10 +3066,10 @@
         <v>177</v>
       </c>
       <c r="B176">
-        <v>2.42</v>
+        <v>3.25</v>
       </c>
       <c r="C176">
-        <v>2.29</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3077,10 +3077,10 @@
         <v>178</v>
       </c>
       <c r="B177">
-        <v>2.39</v>
+        <v>3.27</v>
       </c>
       <c r="C177">
-        <v>2.25</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3088,10 +3088,10 @@
         <v>179</v>
       </c>
       <c r="B178">
-        <v>2.33</v>
+        <v>3.27</v>
       </c>
       <c r="C178">
-        <v>2.19</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -3099,10 +3099,10 @@
         <v>180</v>
       </c>
       <c r="B179">
-        <v>2.31</v>
+        <v>3.2</v>
       </c>
       <c r="C179">
-        <v>2.17</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3110,10 +3110,10 @@
         <v>181</v>
       </c>
       <c r="B180">
-        <v>2.29</v>
+        <v>3.2</v>
       </c>
       <c r="C180">
-        <v>2.14</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3121,10 +3121,10 @@
         <v>182</v>
       </c>
       <c r="B181">
-        <v>2.33</v>
+        <v>3.22</v>
       </c>
       <c r="C181">
-        <v>2.18</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3132,10 +3132,10 @@
         <v>183</v>
       </c>
       <c r="B182">
-        <v>2.31</v>
+        <v>3.21</v>
       </c>
       <c r="C182">
-        <v>2.16</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -3143,10 +3143,10 @@
         <v>184</v>
       </c>
       <c r="B183">
-        <v>2.33</v>
+        <v>3.24</v>
       </c>
       <c r="C183">
-        <v>2.18</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3154,10 +3154,10 @@
         <v>185</v>
       </c>
       <c r="B184">
-        <v>2.29</v>
+        <v>3.3</v>
       </c>
       <c r="C184">
-        <v>2.14</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3165,10 +3165,10 @@
         <v>186</v>
       </c>
       <c r="B185">
-        <v>2.27</v>
+        <v>3.27</v>
       </c>
       <c r="C185">
-        <v>2.13</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3176,10 +3176,10 @@
         <v>187</v>
       </c>
       <c r="B186">
-        <v>2.24</v>
+        <v>3.29</v>
       </c>
       <c r="C186">
-        <v>2.1</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3187,10 +3187,10 @@
         <v>188</v>
       </c>
       <c r="B187">
-        <v>2.31</v>
+        <v>3.33</v>
       </c>
       <c r="C187">
-        <v>2.17</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3198,10 +3198,10 @@
         <v>189</v>
       </c>
       <c r="B188">
-        <v>2.27</v>
+        <v>3.37</v>
       </c>
       <c r="C188">
-        <v>2.13</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3209,10 +3209,10 @@
         <v>190</v>
       </c>
       <c r="B189">
-        <v>2.33</v>
+        <v>3.39</v>
       </c>
       <c r="C189">
-        <v>2.19</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3220,10 +3220,10 @@
         <v>191</v>
       </c>
       <c r="B190">
-        <v>2.34</v>
+        <v>3.34</v>
       </c>
       <c r="C190">
-        <v>2.2</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3231,10 +3231,10 @@
         <v>192</v>
       </c>
       <c r="B191">
-        <v>2.34</v>
+        <v>3.31</v>
       </c>
       <c r="C191">
-        <v>2.2</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3242,10 +3242,10 @@
         <v>193</v>
       </c>
       <c r="B192">
-        <v>2.38</v>
+        <v>3.29</v>
       </c>
       <c r="C192">
-        <v>2.24</v>
+        <v>3.29</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3253,10 +3253,10 @@
         <v>194</v>
       </c>
       <c r="B193">
-        <v>2.34</v>
+        <v>3.25</v>
       </c>
       <c r="C193">
-        <v>2.2</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3264,10 +3264,10 @@
         <v>195</v>
       </c>
       <c r="B194">
-        <v>2.4</v>
+        <v>3.29</v>
       </c>
       <c r="C194">
-        <v>2.26</v>
+        <v>3.29</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3275,10 +3275,10 @@
         <v>196</v>
       </c>
       <c r="B195">
-        <v>2.42</v>
+        <v>3.32</v>
       </c>
       <c r="C195">
-        <v>2.28</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3286,10 +3286,10 @@
         <v>197</v>
       </c>
       <c r="B196">
-        <v>2.39</v>
+        <v>3.31</v>
       </c>
       <c r="C196">
-        <v>2.25</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3297,10 +3297,10 @@
         <v>198</v>
       </c>
       <c r="B197">
-        <v>2.46</v>
+        <v>3.34</v>
       </c>
       <c r="C197">
-        <v>2.32</v>
+        <v>3.34</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3308,10 +3308,10 @@
         <v>199</v>
       </c>
       <c r="B198">
-        <v>2.46</v>
+        <v>3.39</v>
       </c>
       <c r="C198">
-        <v>2.31</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3319,10 +3319,10 @@
         <v>200</v>
       </c>
       <c r="B199">
-        <v>2.41</v>
+        <v>3.39</v>
       </c>
       <c r="C199">
-        <v>2.26</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -3330,10 +3330,10 @@
         <v>201</v>
       </c>
       <c r="B200">
-        <v>2.43</v>
+        <v>3.33</v>
       </c>
       <c r="C200">
-        <v>2.28</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3341,10 +3341,10 @@
         <v>202</v>
       </c>
       <c r="B201">
-        <v>2.47</v>
+        <v>3.34</v>
       </c>
       <c r="C201">
-        <v>2.32</v>
+        <v>3.34</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3352,10 +3352,10 @@
         <v>203</v>
       </c>
       <c r="B202">
-        <v>2.47</v>
+        <v>3.3</v>
       </c>
       <c r="C202">
-        <v>2.33</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -3363,10 +3363,10 @@
         <v>204</v>
       </c>
       <c r="B203">
-        <v>2.48</v>
+        <v>3.31</v>
       </c>
       <c r="C203">
-        <v>2.33</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3374,10 +3374,10 @@
         <v>205</v>
       </c>
       <c r="B204">
-        <v>2.49</v>
+        <v>3.38</v>
       </c>
       <c r="C204">
-        <v>2.34</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -3385,10 +3385,10 @@
         <v>206</v>
       </c>
       <c r="B205">
-        <v>2.44</v>
+        <v>3.42</v>
       </c>
       <c r="C205">
-        <v>2.29</v>
+        <v>3.43</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -3396,10 +3396,10 @@
         <v>207</v>
       </c>
       <c r="B206">
-        <v>2.42</v>
+        <v>3.45</v>
       </c>
       <c r="C206">
-        <v>2.27</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3407,10 +3407,10 @@
         <v>208</v>
       </c>
       <c r="B207">
-        <v>2.37</v>
+        <v>3.44</v>
       </c>
       <c r="C207">
-        <v>2.22</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3418,10 +3418,10 @@
         <v>209</v>
       </c>
       <c r="B208">
-        <v>2.45</v>
+        <v>3.4</v>
       </c>
       <c r="C208">
-        <v>2.3</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -3429,10 +3429,10 @@
         <v>210</v>
       </c>
       <c r="B209">
-        <v>2.44</v>
+        <v>3.36</v>
       </c>
       <c r="C209">
-        <v>2.29</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -3440,10 +3440,10 @@
         <v>211</v>
       </c>
       <c r="B210">
-        <v>2.38</v>
+        <v>3.36</v>
       </c>
       <c r="C210">
-        <v>2.23</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -3451,10 +3451,10 @@
         <v>212</v>
       </c>
       <c r="B211">
-        <v>2.41</v>
+        <v>3.27</v>
       </c>
       <c r="C211">
-        <v>2.27</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -3462,10 +3462,10 @@
         <v>213</v>
       </c>
       <c r="B212">
-        <v>2.42</v>
+        <v>3.31</v>
       </c>
       <c r="C212">
-        <v>2.28</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -3473,10 +3473,10 @@
         <v>214</v>
       </c>
       <c r="B213">
-        <v>2.33</v>
+        <v>3.31</v>
       </c>
       <c r="C213">
-        <v>2.19</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -3484,10 +3484,10 @@
         <v>215</v>
       </c>
       <c r="B214">
-        <v>2.35</v>
+        <v>3.34</v>
       </c>
       <c r="C214">
-        <v>2.2</v>
+        <v>3.34</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -3495,10 +3495,10 @@
         <v>216</v>
       </c>
       <c r="B215">
-        <v>2.29</v>
+        <v>3.37</v>
       </c>
       <c r="C215">
-        <v>2.14</v>
+        <v>3.37</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -3506,10 +3506,10 @@
         <v>217</v>
       </c>
       <c r="B216">
-        <v>2.32</v>
+        <v>3.42</v>
       </c>
       <c r="C216">
-        <v>2.16</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -3517,10 +3517,10 @@
         <v>218</v>
       </c>
       <c r="B217">
-        <v>2.31</v>
+        <v>3.41</v>
       </c>
       <c r="C217">
-        <v>2.16</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -3528,10 +3528,10 @@
         <v>219</v>
       </c>
       <c r="B218">
-        <v>2.34</v>
+        <v>3.44</v>
       </c>
       <c r="C218">
-        <v>2.18</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -3539,10 +3539,10 @@
         <v>220</v>
       </c>
       <c r="B219">
-        <v>2.33</v>
+        <v>3.42</v>
       </c>
       <c r="C219">
-        <v>2.17</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -3550,10 +3550,10 @@
         <v>221</v>
       </c>
       <c r="B220">
-        <v>2.33</v>
+        <v>3.4</v>
       </c>
       <c r="C220">
-        <v>2.17</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -3561,10 +3561,10 @@
         <v>222</v>
       </c>
       <c r="B221">
-        <v>2.39</v>
+        <v>3.41</v>
       </c>
       <c r="C221">
-        <v>2.24</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -3572,10 +3572,10 @@
         <v>223</v>
       </c>
       <c r="B222">
-        <v>2.35</v>
+        <v>3.4</v>
       </c>
       <c r="C222">
-        <v>2.19</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -3583,10 +3583,10 @@
         <v>224</v>
       </c>
       <c r="B223">
-        <v>2.29</v>
+        <v>3.45</v>
       </c>
       <c r="C223">
-        <v>2.15</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -3594,10 +3594,10 @@
         <v>225</v>
       </c>
       <c r="B224">
-        <v>2.19</v>
+        <v>3.41</v>
       </c>
       <c r="C224">
-        <v>2.06</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -3605,10 +3605,10 @@
         <v>226</v>
       </c>
       <c r="B225">
-        <v>2.25</v>
+        <v>3.38</v>
       </c>
       <c r="C225">
-        <v>2.13</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -3616,10 +3616,10 @@
         <v>227</v>
       </c>
       <c r="B226">
-        <v>2.28</v>
+        <v>3.39</v>
       </c>
       <c r="C226">
-        <v>2.16</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -3627,10 +3627,10 @@
         <v>228</v>
       </c>
       <c r="B227">
-        <v>2.29</v>
+        <v>3.39</v>
       </c>
       <c r="C227">
-        <v>2.17</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3638,10 +3638,10 @@
         <v>229</v>
       </c>
       <c r="B228">
-        <v>2.4</v>
+        <v>3.37</v>
       </c>
       <c r="C228">
-        <v>2.27</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3649,10 +3649,10 @@
         <v>230</v>
       </c>
       <c r="B229">
-        <v>2.42</v>
+        <v>3.31</v>
       </c>
       <c r="C229">
-        <v>2.29</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3660,10 +3660,10 @@
         <v>231</v>
       </c>
       <c r="B230">
-        <v>2.43</v>
+        <v>3.27</v>
       </c>
       <c r="C230">
-        <v>2.3</v>
+        <v>3.29</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3671,10 +3671,10 @@
         <v>232</v>
       </c>
       <c r="B231">
-        <v>2.4</v>
+        <v>3.33</v>
       </c>
       <c r="C231">
-        <v>2.27</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3682,10 +3682,10 @@
         <v>233</v>
       </c>
       <c r="B232">
-        <v>2.51</v>
+        <v>3.37</v>
       </c>
       <c r="C232">
-        <v>2.38</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3693,10 +3693,10 @@
         <v>234</v>
       </c>
       <c r="B233">
-        <v>2.48</v>
+        <v>3.34</v>
       </c>
       <c r="C233">
-        <v>2.36</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3704,10 +3704,10 @@
         <v>235</v>
       </c>
       <c r="B234">
-        <v>2.53</v>
+        <v>3.41</v>
       </c>
       <c r="C234">
-        <v>2.41</v>
+        <v>3.43</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3715,10 +3715,10 @@
         <v>236</v>
       </c>
       <c r="B235">
-        <v>2.54</v>
+        <v>3.41</v>
       </c>
       <c r="C235">
-        <v>2.42</v>
+        <v>3.43</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3726,10 +3726,10 @@
         <v>237</v>
       </c>
       <c r="B236">
-        <v>2.53</v>
+        <v>3.38</v>
       </c>
       <c r="C236">
-        <v>2.41</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3737,10 +3737,10 @@
         <v>238</v>
       </c>
       <c r="B237">
-        <v>2.54</v>
+        <v>3.41</v>
       </c>
       <c r="C237">
-        <v>2.42</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3748,10 +3748,10 @@
         <v>239</v>
       </c>
       <c r="B238">
-        <v>2.57</v>
+        <v>3.49</v>
       </c>
       <c r="C238">
-        <v>2.46</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3759,10 +3759,10 @@
         <v>240</v>
       </c>
       <c r="B239">
-        <v>2.54</v>
+        <v>3.47</v>
       </c>
       <c r="C239">
-        <v>2.42</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3770,10 +3770,10 @@
         <v>241</v>
       </c>
       <c r="B240">
-        <v>2.52</v>
+        <v>3.48</v>
       </c>
       <c r="C240">
-        <v>2.41</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3781,10 +3781,10 @@
         <v>242</v>
       </c>
       <c r="B241">
-        <v>2.57</v>
+        <v>3.5</v>
       </c>
       <c r="C241">
-        <v>2.45</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3792,10 +3792,10 @@
         <v>243</v>
       </c>
       <c r="B242">
-        <v>2.55</v>
+        <v>3.53</v>
       </c>
       <c r="C242">
-        <v>2.44</v>
+        <v>3.55</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3803,10 +3803,10 @@
         <v>244</v>
       </c>
       <c r="B243">
-        <v>2.63</v>
+        <v>3.52</v>
       </c>
       <c r="C243">
-        <v>2.51</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3814,10 +3814,10 @@
         <v>245</v>
       </c>
       <c r="B244">
-        <v>2.59</v>
+        <v>3.5</v>
       </c>
       <c r="C244">
-        <v>2.47</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3825,10 +3825,10 @@
         <v>246</v>
       </c>
       <c r="B245">
-        <v>2.63</v>
+        <v>3.52</v>
       </c>
       <c r="C245">
-        <v>2.51</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3836,10 +3836,10 @@
         <v>247</v>
       </c>
       <c r="B246">
-        <v>2.7</v>
+        <v>3.61</v>
       </c>
       <c r="C246">
-        <v>2.59</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3847,10 +3847,10 @@
         <v>248</v>
       </c>
       <c r="B247">
-        <v>2.66</v>
+        <v>3.64</v>
       </c>
       <c r="C247">
-        <v>2.55</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3858,10 +3858,10 @@
         <v>249</v>
       </c>
       <c r="B248">
-        <v>2.68</v>
+        <v>3.61</v>
       </c>
       <c r="C248">
-        <v>2.56</v>
+        <v>3.64</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3869,10 +3869,10 @@
         <v>250</v>
       </c>
       <c r="B249">
-        <v>2.7</v>
+        <v>3.63</v>
       </c>
       <c r="C249">
-        <v>2.59</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3880,10 +3880,10 @@
         <v>251</v>
       </c>
       <c r="B250">
-        <v>2.77</v>
+        <v>3.66</v>
       </c>
       <c r="C250">
-        <v>2.67</v>
+        <v>3.69</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3891,10 +3891,10 @@
         <v>252</v>
       </c>
       <c r="B251">
-        <v>2.75</v>
+        <v>3.66</v>
       </c>
       <c r="C251">
-        <v>2.64</v>
+        <v>3.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>